<commit_message>
Reorganización de análisis en carpetas y subcarpetas creadas
</commit_message>
<xml_diff>
--- a/Modelizacion/Clustering_oro_por_minuto_NO_UTILITY.xlsx
+++ b/Modelizacion/Clustering_oro_por_minuto_NO_UTILITY.xlsx
@@ -3257,7 +3257,7 @@
         <v>10</v>
       </c>
       <c r="G80" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81">
@@ -4798,7 +4798,7 @@
         <v>8</v>
       </c>
       <c r="G147" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="148">
@@ -5005,7 +5005,7 @@
         <v>8</v>
       </c>
       <c r="G156" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="157">

</xml_diff>

<commit_message>
install libraries (Nlme, lme4, stargazer, emmeans, kableExtra, purrr)
Created files "Clustering_Select_Variables" and "Modelos Mixtos"

Section 6.2.2 --> Clustering with golearned, champExperience, assits, etc

Section 6.3. --> Modelos Mixtos
</commit_message>
<xml_diff>
--- a/Modelizacion/Clustering_oro_por_minuto_NO_UTILITY.xlsx
+++ b/Modelizacion/Clustering_oro_por_minuto_NO_UTILITY.xlsx
@@ -3257,7 +3257,7 @@
         <v>10</v>
       </c>
       <c r="G80" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81">
@@ -4798,7 +4798,7 @@
         <v>8</v>
       </c>
       <c r="G147" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148">
@@ -5005,7 +5005,7 @@
         <v>8</v>
       </c>
       <c r="G156" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="157">

</xml_diff>